<commit_message>
Added Config data provider
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ganesh Bhoge\eclipse-workspace\Vault\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA743734-8F32-4898-B234-46D36E1BA45D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{AC6F8FBE-CF49-490B-A29A-953094111976}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6230" xr2:uid="{5F650742-CECE-4D66-A56D-221D4FAB16BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14180" windowHeight="3360" xr2:uid="{5F650742-CECE-4D66-A56D-221D4FAB16BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -396,7 +392,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>